<commit_message>
connection jdbc to target DB for metadata
</commit_message>
<xml_diff>
--- a/column.xlsx
+++ b/column.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\workspace\springboot_react\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6A3333-422C-46AF-BE75-D9982827BCD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50216E23-D42E-48B0-B167-FE688A64FBEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10403" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10403" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="1" r:id="rId1"/>
@@ -19982,7 +19982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1524"/>
   <sheetViews>
-    <sheetView topLeftCell="B799" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="D804" sqref="D804"/>
     </sheetView>
   </sheetViews>
@@ -78263,11 +78263,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D414CD-452D-4B9E-8D10-02680BEB590D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M157"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G157"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -79594,7 +79593,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A60">
         <v>59</v>
       </c>
@@ -79689,7 +79688,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A64">
         <v>63</v>
       </c>
@@ -79715,7 +79714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A65">
         <v>64</v>
       </c>
@@ -79741,7 +79740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A66">
         <v>65</v>
       </c>
@@ -80319,7 +80318,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A91">
         <v>90</v>
       </c>
@@ -80345,7 +80344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A92">
         <v>91</v>
       </c>
@@ -80371,7 +80370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A93">
         <v>92</v>
       </c>
@@ -80397,7 +80396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A94">
         <v>93</v>
       </c>
@@ -80423,7 +80422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A95">
         <v>94</v>
       </c>
@@ -80587,7 +80586,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A102">
         <v>101</v>
       </c>
@@ -80604,7 +80603,7 @@
         <v>4619</v>
       </c>
     </row>
-    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A103">
         <v>102</v>
       </c>
@@ -80622,7 +80621,7 @@
       </c>
       <c r="M103" s="9"/>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A104">
         <v>103</v>
       </c>
@@ -80800,7 +80799,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.6">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A112">
         <v>111</v>
       </c>
@@ -80964,7 +80963,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A119">
         <v>118</v>
       </c>
@@ -81013,7 +81012,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A121">
         <v>120</v>
       </c>
@@ -81039,7 +81038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A122">
         <v>121</v>
       </c>
@@ -81065,7 +81064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A123">
         <v>122</v>
       </c>
@@ -81091,7 +81090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A124">
         <v>123</v>
       </c>
@@ -81117,7 +81116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A125">
         <v>124</v>
       </c>
@@ -81143,7 +81142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A126">
         <v>125</v>
       </c>
@@ -81468,7 +81467,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A140">
         <v>139</v>
       </c>
@@ -81793,7 +81792,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A154">
         <v>153</v>
       </c>
@@ -81819,7 +81818,7 @@
         <v>4618</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.6">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A155">
         <v>154</v>
       </c>
@@ -81892,11 +81891,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N157" xr:uid="{40C8E0B3-4BF0-4752-B839-F88CE852CDAF}">
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N157" xr:uid="{40C8E0B3-4BF0-4752-B839-F88CE852CDAF}"/>
   <sortState ref="C2:F157">
     <sortCondition ref="C2:C157"/>
     <sortCondition ref="F2:F157"/>
@@ -81910,7 +81905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCF9FCA-73D2-41E7-9D00-D2EFF5C2AEF4}">
   <dimension ref="A2:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>

</xml_diff>